<commit_message>
plotted alpha diversity means and sds and updated alpha div modeling a bit
</commit_message>
<xml_diff>
--- a/Test output for alpha div models.xlsx
+++ b/Test output for alpha div models.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="0" windowWidth="13420" windowHeight="11660" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-30920" yWindow="460" windowWidth="25360" windowHeight="14280" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Evenness" sheetId="1" r:id="rId1"/>
     <sheet name="Shannons" sheetId="2" r:id="rId2"/>
     <sheet name="RIchness" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="39">
   <si>
     <t>Pathotype_1</t>
   </si>
@@ -89,7 +90,55 @@
     <t xml:space="preserve">Pathotype_1 </t>
   </si>
   <si>
-    <t>33-6</t>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Pathotype</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Ever vs Never</t>
+  </si>
+  <si>
+    <t>Never Shed</t>
+  </si>
+  <si>
+    <t>Shed at least once</t>
+  </si>
+  <si>
+    <t>Multi-Day Shedder</t>
+  </si>
+  <si>
+    <t>Intermittent Shedder</t>
+  </si>
+  <si>
+    <t>EHEC/aEPEC sample</t>
+  </si>
+  <si>
+    <t>Non-O157 Sample</t>
+  </si>
+  <si>
+    <t>alpha_measure</t>
+  </si>
+  <si>
+    <t>Evenness</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Richness</t>
+  </si>
+  <si>
+    <t>Shannons</t>
   </si>
 </sst>
 </file>
@@ -164,8 +213,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -197,7 +272,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -209,6 +284,19 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -220,6 +308,19 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -551,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -920,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1280,7 +1381,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1472,8 +1573,8 @@
       <c r="E21">
         <v>-1653</v>
       </c>
-      <c r="F21" t="s">
-        <v>22</v>
+      <c r="F21">
+        <v>3306</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1622,6 +1723,410 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>0.73775679999999999</v>
+      </c>
+      <c r="E2">
+        <v>2.944107E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>0.74294559999999998</v>
+      </c>
+      <c r="E3">
+        <v>3.1162169999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>0.73676620000000004</v>
+      </c>
+      <c r="E4">
+        <v>3.0212180000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>0.73792630000000003</v>
+      </c>
+      <c r="E5">
+        <v>2.5476809999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>0.74901879999999998</v>
+      </c>
+      <c r="E6">
+        <v>3.6192099999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>0.73676620000000004</v>
+      </c>
+      <c r="E7">
+        <v>3.0212180000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>0.74073449999999996</v>
+      </c>
+      <c r="E8">
+        <v>2.8727570000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>4184.04</v>
+      </c>
+      <c r="E9">
+        <v>1132.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10">
+        <v>4126.174</v>
+      </c>
+      <c r="E10">
+        <v>1725.664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <v>4206.3249999999998</v>
+      </c>
+      <c r="E11">
+        <v>964.70799999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12">
+        <v>4250.3900000000003</v>
+      </c>
+      <c r="E12">
+        <v>1557.9690000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13">
+        <v>3791.4</v>
+      </c>
+      <c r="E13">
+        <v>1335.271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <v>4206.3249999999998</v>
+      </c>
+      <c r="E14">
+        <v>964.70799999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>4134.1899999999996</v>
+      </c>
+      <c r="E15">
+        <v>1509.8150000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>6.1123589999999997</v>
+      </c>
+      <c r="E16">
+        <v>0.32952680000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>6.1234979999999997</v>
+      </c>
+      <c r="E17">
+        <v>0.40001009999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>6.1219640000000002</v>
+      </c>
+      <c r="E18">
+        <v>0.30857210000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <v>6.0983749999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.30313040000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>6.1102359999999996</v>
+      </c>
+      <c r="E20">
+        <v>0.55265310000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>6.1219640000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.30857210000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>6.1013780000000004</v>
+      </c>
+      <c r="E22">
+        <v>0.37782589999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>